<commit_message>
Algorithm study Commit - DFS
</commit_message>
<xml_diff>
--- a/알고리즘 계획표.xlsx
+++ b/알고리즘 계획표.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JAVA\projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\IdeaProjects\AlgorithmStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E957D430-FBFF-4F7D-AFEA-301216197B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="계획표" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>문제번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,113 +59,122 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>탐색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS/BFS (한 문제는 꼭 나옴)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9012 (스택 &amp; 문자열)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2164 (큐) 문제에서 FIFO 파악 poll, peek, add 메소드 용도 파악</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10773 (스택) 문제에서 LIFO 파악, push, pop 메소드 용도 파악</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10845 (큐) - Queue클래스 메소드, 전역, 지역변수, StringTokenizer 개념 숙지하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해싱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파싱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>힙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS/BFS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(한 문제는 꼭 나옴!)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP(Dynamic Programming)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1158 (큐)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1120 (문자열)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11724 (DFS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탐색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>백준 10816, 백준 1439, 백준 10799, 백준 1992, 백준 9012, 백준 2447, 백준 10101, 백준 14503, 백준 3040, 백준 11403, 백준 11651, 백준 1789, 백준 15649, 백준 15650, 백준 11497, 프로그래머스 42895, 백준 9663, 백준 2630, 백준 1446, 백준 1094, 백준 4307, 백준 4485, 백준 1520, 백준 9084, 백준 11758, 백준 1991, 백준 17779, 백준 11053, 백준 13869, 백준 9251, 백준 1766, 백준 11725, 백준 10845, 백준 1004, 백준 4256, 백준 11724, 백준 1337, 백준 7490, 백준 2022, 백준 1340, 백준 17140, 백준 1389, 백준 1158, 백준 1316, 백준 10815, 백준 17266, 백준 7795, 백준 11054, 백준 8958, 백준 7576, 백준 1912, 백준 9020, 백준 16236, 백준 1167, 백준 2437, 백준 15686, 백준 9095, 백준 1194, 백준 25644, 백준 2170, 백준 1922, 백준 17070, 백준 1525, 백준 18352, 백준 1918, 백준 14725, 백준 7569, 백준 2887, 백준 12015, 백준 1007, 백준 1197, 백준 10942, 백준 1509, 백준 1194, 백준 1562, 백준 1799</t>
-  </si>
-  <si>
-    <t>탐색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DFS/BFS (한 문제는 꼭 나옴)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그리디</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9012 (스택 &amp; 문자열)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2164 (큐) 문제에서 FIFO 파악 poll, peek, add 메소드 용도 파악</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10773 (스택) 문제에서 LIFO 파악, push, pop 메소드 용도 파악</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10845 (큐) - Queue클래스 메소드, 전역, 지역변수, StringTokenizer 개념 숙지하기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해싱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파싱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>힙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>트리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>문자열</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DFS/BFS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(한 문제는 꼭 나옴!)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DP(Dynamic Programming)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>종류</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1158 (큐)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1120 (문자열)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -245,7 +253,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -271,6 +279,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -598,11 +609,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -618,16 +629,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -646,21 +657,21 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>240430</v>
@@ -682,9 +693,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2">
         <v>240502</v>
@@ -706,9 +717,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2">
         <v>240502</v>
@@ -730,9 +741,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2">
         <v>240507</v>
@@ -741,10 +752,10 @@
         <v>240508</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="2">
         <v>240517</v>
@@ -754,9 +765,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2">
         <v>240517</v>
@@ -770,9 +781,9 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2">
         <v>240517</v>
@@ -785,23 +796,26 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <v>11724</v>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="9">
+        <v>240522</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
+      <c r="A10" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -816,7 +830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7DE8D4-55D6-4D0F-A0F0-BE830A70EFFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -831,80 +845,80 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+      <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -917,7 +931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -929,7 +943,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Algorithm study Commit - BFS 핵심이론 커밋
</commit_message>
<xml_diff>
--- a/알고리즘 계획표.xlsx
+++ b/알고리즘 계획표.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>문제번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -111,10 +111,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>스택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>힙</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -168,6 +164,14 @@
   </si>
   <si>
     <t>백준 10816, 백준 1439, 백준 10799, 백준 1992, 백준 9012, 백준 2447, 백준 10101, 백준 14503, 백준 3040, 백준 11403, 백준 11651, 백준 1789, 백준 15649, 백준 15650, 백준 11497, 프로그래머스 42895, 백준 9663, 백준 2630, 백준 1446, 백준 1094, 백준 4307, 백준 4485, 백준 1520, 백준 9084, 백준 11758, 백준 1991, 백준 17779, 백준 11053, 백준 13869, 백준 9251, 백준 1766, 백준 11725, 백준 10845, 백준 1004, 백준 4256, 백준 11724, 백준 1337, 백준 7490, 백준 2022, 백준 1340, 백준 17140, 백준 1389, 백준 1158, 백준 1316, 백준 10815, 백준 17266, 백준 7795, 백준 11054, 백준 8958, 백준 7576, 백준 1912, 백준 9020, 백준 16236, 백준 1167, 백준 2437, 백준 15686, 백준 9095, 백준 1194, 백준 25644, 백준 2170, 백준 1922, 백준 17070, 백준 1525, 백준 18352, 백준 1918, 백준 14725, 백준 7569, 백준 2887, 백준 12015, 백준 1007, 백준 1197, 백준 10942, 백준 1509, 백준 1194, 백준 1562, 백준 1799</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2178 (BFS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스택/큐</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -253,7 +257,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -279,6 +283,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -610,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -629,16 +639,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -667,7 +677,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -693,7 +703,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
@@ -717,7 +727,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
@@ -741,7 +751,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -752,10 +762,10 @@
         <v>240508</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2">
         <v>240517</v>
@@ -765,9 +775,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2">
         <v>240517</v>
@@ -781,9 +791,9 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2">
         <v>240517</v>
@@ -793,35 +803,45 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="9">
         <v>240522</v>
       </c>
+      <c r="D9" s="10">
+        <v>240523</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>33</v>
+      <c r="A10" s="14"/>
+      <c r="B10" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
+      <c r="A11" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -834,7 +854,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -845,10 +865,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -856,11 +876,11 @@
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -868,41 +888,41 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+      <c r="B8" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -910,15 +930,15 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +963,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Algorithm study Commit - BFS 및 DFS 커밋
</commit_message>
<xml_diff>
--- a/알고리즘 계획표.xlsx
+++ b/알고리즘 계획표.xlsx
@@ -167,11 +167,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2178 (BFS)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>스택/큐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1260 (DFS/BFS 뼈대문제임 잘 숙지하기!)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -257,7 +257,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -283,6 +283,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -623,7 +629,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -639,16 +645,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -677,7 +683,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -703,7 +709,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
@@ -727,7 +733,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
@@ -751,7 +757,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -775,7 +781,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
@@ -785,13 +791,15 @@
       <c r="D7" s="2">
         <v>240521</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="13">
+        <v>240524</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
@@ -803,7 +811,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -817,9 +825,12 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="C10" s="12">
+        <v>240524</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -880,7 +891,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -888,31 +899,31 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="4" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Algorithm Study - 10026, 2468번 문제 분석 시트 추가
</commit_message>
<xml_diff>
--- a/알고리즘 계획표.xlsx
+++ b/알고리즘 계획표.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JAVA\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B41C47B-F2B5-440C-90BD-C460A9080117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE5A96A-EDA5-43C8-9ED8-3F9DEA6C2469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="계획표" sheetId="1" r:id="rId1"/>
-    <sheet name="빈출유형" sheetId="3" r:id="rId2"/>
-    <sheet name="헤이밥 추천 백준 문제들 (참고용)" sheetId="2" r:id="rId3"/>
+    <sheet name="10026&lt;-&gt;2468" sheetId="4" r:id="rId2"/>
+    <sheet name="빈출유형" sheetId="3" r:id="rId3"/>
+    <sheet name="헤이밥 추천 백준 문제들 (참고용)" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -87,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>문제번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -292,11 +293,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10026(DFS/BFS 둘 다 풀이 가능)
-미로형식 문제, 미로형식 문제에서 0, 1 그 이상의 종류가 오면 어떻게 처리할 것인지 파악</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DFS/BFS
 (그래프형식 / 미로형식 문제 잘 파악해서 풀기)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -332,7 +328,290 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2468(미로탐색에서 범위로 탐색하는 방법 익히기)</t>
+    <t>10026(DFS/BFS 둘 다 풀이 가능)
+미로형식 문제, 미로형식 문제에서 0, 1 그 이상의 종류가 오면 어떻게 처리할 것인지 파악</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2468(미로탐색 -&gt; 탐색 가능 지역이 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'특정값 이상'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">일때 로직 생각하면서 코딩하기)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-&gt; 10026번 문제랑은 다르게 생각해야함.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문제유형</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>접근법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BFS(미로탐색)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공통점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차이점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 미로에 0과 1외 2가지 이상의 요소가존재
+- BFS 함수 파라미터로 i, j 좌표 외에 해당 요소가 추가됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>★ 요소의 종류가 많아 for문으로 구현</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>★</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 특정 요소를 기준으로한 특정범위</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">로 접근
+        ex) 지형높이가 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 이상</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>인 지형을 탐색</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 미로[i][j] = '요소의 종류' &amp;&amp; !visited[i][j] 조건으로 loop 돌림 (기존 미로탐색 loop)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 미로를 구성하는 요소의 최솟값과 최댓값을 구한 후 그 사이의 값을 최상단 loop로 돌면서 그 안에 기존 미로탐색 loop를 돌린다.
+- 미로[i][j] &gt;= '요소의 종류' &amp;&amp; !visited[i][j] 조건으로 loop 돌림 (기존 미로탐색 loop)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>★</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 요소의 종류가 3개밖에 되지 않아 if문으로 구현</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+★</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">특정 범위가 아닌 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>요소의 종류</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">로 접근
+        ex) 적록색약인 경우 빨간색과 초록색을 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>빨간색</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>으로 통일하고 탐색
+             따라서</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 빨간색과 파란색인 구역</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>만 탐색</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -340,7 +619,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,6 +683,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -448,7 +742,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -496,6 +790,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,11 +1122,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="2" width="35.875" customWidth="1"/>
     <col min="3" max="3" width="83.375" bestFit="1" customWidth="1"/>
@@ -831,7 +1140,7 @@
     <col min="11" max="11" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="96" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -844,7 +1153,7 @@
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -877,7 +1186,7 @@
       </c>
       <c r="K2" s="13"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -912,7 +1221,7 @@
         <v>240612</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
@@ -943,7 +1252,7 @@
         <v>240612</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="2" t="s">
@@ -974,7 +1283,7 @@
         <v>240612</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="33">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="7" t="s">
@@ -1005,7 +1314,7 @@
         <v>240612</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="2" t="s">
@@ -1033,7 +1342,7 @@
         <v>240612</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>41</v>
@@ -1063,7 +1372,7 @@
         <v>240612</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>42</v>
@@ -1087,12 +1396,12 @@
         <v>240617</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="16.5" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>29</v>
@@ -1122,7 +1431,7 @@
         <v>240705</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11" s="10"/>
       <c r="B11" s="14"/>
       <c r="C11" s="2" t="s">
@@ -1150,7 +1459,7 @@
         <v>240618</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12" s="10"/>
       <c r="B12" s="14"/>
       <c r="C12" s="2" t="s">
@@ -1181,7 +1490,7 @@
         <v>240705</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="A13" s="10"/>
       <c r="B13" s="14"/>
       <c r="C13" s="2" t="s">
@@ -1212,11 +1521,11 @@
         <v>240709</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="49.5">
       <c r="A14" s="10"/>
       <c r="B14" s="14"/>
       <c r="C14" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="2">
         <v>240613</v>
@@ -1238,11 +1547,11 @@
       </c>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="33">
       <c r="A15" s="10"/>
       <c r="B15" s="14"/>
       <c r="C15" s="7" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D15" s="8">
         <v>240618</v>
@@ -1260,11 +1569,11 @@
         <v>240705</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16" s="10"/>
       <c r="B16" s="14"/>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="8">
         <v>240710</v>
@@ -1276,17 +1585,17 @@
         <v>240713</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="33">
       <c r="A17" s="10"/>
       <c r="B17" s="14"/>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="8">
         <v>240716</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="33">
       <c r="A18" s="10" t="s">
         <v>37</v>
       </c>
@@ -1315,7 +1624,7 @@
         <v>240709</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="2" t="s">
@@ -1335,11 +1644,11 @@
       </c>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="8">
         <v>240619</v>
@@ -1357,11 +1666,11 @@
         <v>240709</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="8">
         <v>240619</v>
@@ -1376,12 +1685,12 @@
         <v>240628</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2">
         <v>11047</v>
@@ -1399,27 +1708,29 @@
         <v>240716</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="8">
         <v>240716</v>
       </c>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="J2:K2"/>
@@ -1428,8 +1739,6 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="B10:B17"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1439,6 +1748,81 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0DB155-46BC-46D7-A350-72EC5C006E27}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.625" customWidth="1"/>
+    <col min="4" max="4" width="67.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="83.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="66">
+      <c r="A2" s="2">
+        <v>10026</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="59.25" customHeight="1">
+      <c r="A3" s="2">
+        <v>2468</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:C3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1446,13 +1830,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
@@ -1460,7 +1844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1468,7 +1852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
@@ -1476,37 +1860,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="15"/>
       <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="15"/>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="15"/>
       <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="15"/>
       <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -1514,7 +1898,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1522,7 +1906,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1539,18 +1923,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="255.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Algorithm Study - 백준 : 1260 DFS와 BFS 알고리즘 일정표 업데이트
</commit_message>
<xml_diff>
--- a/알고리즘 계획표.xlsx
+++ b/알고리즘 계획표.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JAVA\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7DB2C7-24A2-453F-A8D2-77CF324B7591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411F4252-D5C9-4A64-B515-8D19F01E9E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -939,20 +939,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1285,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -1304,17 +1304,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="96" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
@@ -1344,16 +1344,16 @@
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="18"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1385,8 +1385,8 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1416,8 +1416,8 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1447,8 +1447,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="7" t="s">
         <v>39</v>
       </c>
@@ -1478,8 +1478,8 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1506,8 +1506,8 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="2" t="s">
         <v>76</v>
       </c>
@@ -1528,8 +1528,8 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="33">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="7" t="s">
         <v>79</v>
       </c>
@@ -1550,7 +1550,7 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="15"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
@@ -1580,7 +1580,7 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="15"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
@@ -1604,10 +1604,10 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>84</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1639,8 +1639,8 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="15"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1665,10 +1665,13 @@
       <c r="J13" s="2">
         <v>240618</v>
       </c>
+      <c r="K13" s="2">
+        <v>240824</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="15"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
@@ -1698,8 +1701,8 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="15"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="2" t="s">
         <v>35</v>
       </c>
@@ -1729,8 +1732,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="49.5">
-      <c r="A16" s="15"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="7" t="s">
         <v>48</v>
       </c>
@@ -1755,8 +1758,8 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" ht="33">
-      <c r="A17" s="15"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="7" t="s">
         <v>53</v>
       </c>
@@ -1780,8 +1783,8 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="15"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="2" t="s">
         <v>50</v>
       </c>
@@ -1805,8 +1808,8 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="33">
-      <c r="A19" s="15"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="7" t="s">
         <v>54</v>
       </c>
@@ -1830,8 +1833,8 @@
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="15"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="7">
         <v>4963</v>
       </c>
@@ -1851,8 +1854,8 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="15"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="7" t="s">
         <v>85</v>
       </c>
@@ -1868,10 +1871,10 @@
       <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="33">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1900,8 +1903,8 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1920,8 +1923,8 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="2" t="s">
         <v>46</v>
       </c>
@@ -1948,8 +1951,8 @@
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="2" t="s">
         <v>47</v>
       </c>
@@ -1964,10 +1967,10 @@
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="2">
@@ -1990,8 +1993,8 @@
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2" t="s">
         <v>52</v>
       </c>
@@ -2012,8 +2015,8 @@
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="2" t="s">
         <v>80</v>
       </c>
@@ -2038,7 +2041,7 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="16" t="s">
         <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -2064,8 +2067,8 @@
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15" t="s">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16" t="s">
         <v>75</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -2088,8 +2091,8 @@
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="2">
         <v>1427</v>
       </c>
@@ -2107,7 +2110,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="15"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="2" t="s">
         <v>82</v>
       </c>
@@ -2128,10 +2131,10 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -2151,8 +2154,8 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="2" t="s">
         <v>81</v>
       </c>
@@ -2168,6 +2171,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A30:A33"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
@@ -2176,12 +2185,6 @@
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="A12:A21"/>
     <mergeCell ref="B12:B21"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A30:A33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2247,7 +2250,7 @@
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="11" t="s">
         <v>61</v>
       </c>

</xml_diff>